<commit_message>
Update new task sheet for report 1
</commit_message>
<xml_diff>
--- a/Documents/C2B_TasksheetFinal.xlsx
+++ b/Documents/C2B_TasksheetFinal.xlsx
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>No.</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>Review Report 1</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -579,13 +582,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -601,6 +597,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -952,10 +956,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="25">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -971,12 +975,14 @@
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>75</v>
@@ -986,12 +992,14 @@
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
         <v>75</v>
@@ -1001,28 +1009,36 @@
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>75</v>
@@ -1031,13 +1047,17 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
         <v>75</v>
@@ -1046,12 +1066,14 @@
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="24" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>75</v>
       </c>
@@ -1061,27 +1083,35 @@
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="26">
-        <v>2</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="30">
+        <v>2</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1091,10 +1121,10 @@
       <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1104,10 +1134,10 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="15.75">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1117,10 +1147,10 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="15.75">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1130,14 +1160,10 @@
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="15.75">
-      <c r="A14" s="26">
-        <v>3</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>5</v>
-      </c>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1147,10 +1173,14 @@
       <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15.75">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="5" t="s">
-        <v>14</v>
+      <c r="A15" s="30">
+        <v>3</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1160,10 +1190,10 @@
       <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="15.75">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="6" t="s">
-        <v>15</v>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1173,10 +1203,10 @@
       <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="15.75">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="7" t="s">
-        <v>16</v>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1186,10 +1216,10 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="8" t="s">
-        <v>18</v>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1199,10 +1229,10 @@
       <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1212,10 +1242,10 @@
       <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1225,10 +1255,10 @@
       <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="7" t="s">
-        <v>21</v>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1238,10 +1268,10 @@
       <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="8" t="s">
-        <v>22</v>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1251,10 +1281,10 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1264,10 +1294,10 @@
       <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1277,10 +1307,10 @@
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="9" t="s">
-        <v>25</v>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1290,14 +1320,10 @@
       <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="30">
-        <v>4</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>26</v>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1307,10 +1333,14 @@
       <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="27">
+        <v>4</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="C27" s="4" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1320,10 +1350,10 @@
       <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" ht="15.75">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="10" t="s">
-        <v>51</v>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1333,10 +1363,10 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="11" t="s">
-        <v>52</v>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1346,10 +1376,10 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" ht="15.75">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1359,10 +1389,10 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="12" t="s">
-        <v>27</v>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1372,10 +1402,10 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="10" t="s">
-        <v>28</v>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1385,10 +1415,10 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="11" t="s">
-        <v>29</v>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1398,10 +1428,10 @@
       <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1411,10 +1441,10 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="13" t="s">
-        <v>31</v>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1424,10 +1454,10 @@
       <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" ht="15.75">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="8" t="s">
-        <v>47</v>
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1437,10 +1467,10 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1450,10 +1480,10 @@
       <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1463,10 +1493,10 @@
       <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="13" t="s">
-        <v>45</v>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1476,10 +1506,10 @@
       <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1489,14 +1519,10 @@
       <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="27">
-        <v>5</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>40</v>
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1506,10 +1532,14 @@
       <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="28"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="24">
+        <v>5</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="C42" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1519,10 +1549,10 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="28"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="11" t="s">
-        <v>34</v>
+      <c r="A43" s="25"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1532,10 +1562,10 @@
       <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="28"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1545,10 +1575,10 @@
       <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="28"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="5" t="s">
-        <v>33</v>
+      <c r="A45" s="25"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1558,10 +1588,10 @@
       <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="28"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="11" t="s">
-        <v>34</v>
+      <c r="A46" s="25"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1571,10 +1601,10 @@
       <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="28"/>
-      <c r="B47" s="26"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1584,10 +1614,10 @@
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="28"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="4" t="s">
-        <v>56</v>
+      <c r="A48" s="25"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1597,10 +1627,10 @@
       <c r="I48" s="15"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
-      <c r="A49" s="28"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="13" t="s">
-        <v>36</v>
+      <c r="A49" s="25"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1610,10 +1640,10 @@
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="28"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="11" t="s">
-        <v>17</v>
+      <c r="A50" s="25"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1623,10 +1653,10 @@
       <c r="I50" s="15"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
-      <c r="A51" s="28"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="11" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1636,10 +1666,10 @@
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
-      <c r="A52" s="28"/>
-      <c r="B52" s="26"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1649,10 +1679,10 @@
       <c r="I52" s="15"/>
     </row>
     <row r="53" spans="1:9" ht="15.75">
-      <c r="A53" s="28"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="13" t="s">
-        <v>37</v>
+      <c r="A53" s="25"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1662,10 +1692,10 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
-      <c r="A54" s="28"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="11" t="s">
-        <v>17</v>
+      <c r="A54" s="25"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1675,10 +1705,10 @@
       <c r="I54" s="15"/>
     </row>
     <row r="55" spans="1:9" ht="15.75">
-      <c r="A55" s="28"/>
-      <c r="B55" s="26"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="11" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1688,10 +1718,10 @@
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" ht="15.75">
-      <c r="A56" s="28"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="13" t="s">
-        <v>54</v>
+      <c r="A56" s="25"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1701,10 +1731,10 @@
       <c r="I56" s="15"/>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="28"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="11" t="s">
-        <v>17</v>
+      <c r="A57" s="25"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1714,10 +1744,10 @@
       <c r="I57" s="15"/>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="29"/>
-      <c r="B58" s="26"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="30"/>
       <c r="C58" s="11" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1727,14 +1757,10 @@
       <c r="I58" s="15"/>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="27">
-        <v>6</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>41</v>
+      <c r="A59" s="26"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1744,10 +1770,14 @@
       <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="28"/>
-      <c r="B60" s="31"/>
+      <c r="A60" s="24">
+        <v>6</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="C60" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1757,10 +1787,10 @@
       <c r="I60" s="15"/>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="28"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="11" t="s">
-        <v>17</v>
+      <c r="A61" s="25"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1770,10 +1800,10 @@
       <c r="I61" s="15"/>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="28"/>
-      <c r="B62" s="31"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="11" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1783,10 +1813,10 @@
       <c r="I62" s="15"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="28"/>
-      <c r="B63" s="31"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1796,10 +1826,10 @@
       <c r="I63" s="15"/>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="29"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="13" t="s">
-        <v>43</v>
+      <c r="A64" s="25"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -1808,20 +1838,21 @@
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
     </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="I65" s="3"/>
+    <row r="65" spans="1:9" ht="15.75">
+      <c r="A65" s="26"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="20" t="s">
-        <v>59</v>
-      </c>
+      <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="1"/>
       <c r="D66" s="3"/>
@@ -1831,30 +1862,26 @@
       <c r="I66" s="3"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="A67" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="1"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="I67" s="3"/>
     </row>
-    <row r="68" spans="1:9" ht="60">
-      <c r="A68" s="21">
-        <v>1</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="4">
-        <v>1</v>
+    <row r="68" spans="1:9">
+      <c r="A68" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -1862,15 +1889,15 @@
       <c r="G68" s="3"/>
       <c r="I68" s="3"/>
     </row>
-    <row r="69" spans="1:9" ht="30">
-      <c r="A69" s="23">
-        <v>2</v>
+    <row r="69" spans="1:9" ht="60">
+      <c r="A69" s="21">
+        <v>1</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C69" s="23">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="C69" s="4">
+        <v>1</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -1880,13 +1907,13 @@
     </row>
     <row r="70" spans="1:9" ht="30">
       <c r="A70" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C70" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -1896,13 +1923,13 @@
     </row>
     <row r="71" spans="1:9" ht="30">
       <c r="A71" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C71" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -1912,13 +1939,13 @@
     </row>
     <row r="72" spans="1:9" ht="30">
       <c r="A72" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C72" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -1926,7 +1953,16 @@
       <c r="G72" s="3"/>
       <c r="I72" s="3"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" ht="30">
+      <c r="A73" s="23">
+        <v>5</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C73" s="23">
+        <v>5</v>
+      </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -2031,23 +2067,30 @@
       <c r="G87" s="3"/>
       <c r="I87" s="3"/>
     </row>
+    <row r="88" spans="4:9">
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="I88" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="B59:B64"/>
-    <mergeCell ref="B41:B58"/>
-    <mergeCell ref="A41:A58"/>
-    <mergeCell ref="B26:B40"/>
-    <mergeCell ref="A26:A40"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="B60:B65"/>
+    <mergeCell ref="B42:B59"/>
+    <mergeCell ref="A42:A59"/>
+    <mergeCell ref="B27:B41"/>
+    <mergeCell ref="A27:A41"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G86">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Report 2 + Task Sheet Report 2
</commit_message>
<xml_diff>
--- a/Documents/C2B_TasksheetFinal.xlsx
+++ b/Documents/C2B_TasksheetFinal.xlsx
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
   <si>
     <t>No.</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Project management plan</t>
   </si>
   <si>
-    <t>…..</t>
-  </si>
-  <si>
     <t>Coding Convention</t>
   </si>
   <si>
@@ -358,6 +355,36 @@
   </si>
   <si>
     <t>Review Report 1</t>
+  </si>
+  <si>
+    <t>_Name of this Capstone Project</t>
+  </si>
+  <si>
+    <t>_Problem Abstract</t>
+  </si>
+  <si>
+    <t>_Project Overview</t>
+  </si>
+  <si>
+    <t>_Software Process Model</t>
+  </si>
+  <si>
+    <t>_Roles and responsibilities</t>
+  </si>
+  <si>
+    <t>_Tools and Techniques</t>
+  </si>
+  <si>
+    <t>Review Report 2</t>
+  </si>
+  <si>
+    <t>_Software development life cycle</t>
+  </si>
+  <si>
+    <t>_Phase Detail</t>
+  </si>
+  <si>
+    <t>_All Meeting Minutes</t>
   </si>
 </sst>
 </file>
@@ -582,6 +609,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -597,14 +632,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -937,36 +964,36 @@
         <v>2</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>70</v>
-      </c>
       <c r="H1" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="29">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -975,143 +1002,143 @@
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
-        <v>74</v>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="32" t="s">
-        <v>76</v>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="25" t="s">
+        <v>75</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="30">
+      <c r="A10" s="27">
         <v>2</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1121,10 +1148,10 @@
       <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="4" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1134,10 +1161,10 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="15.75">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="4" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1147,10 +1174,10 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="15.75">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1160,10 +1187,10 @@
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="15.75">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1173,14 +1200,10 @@
       <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15.75">
-      <c r="A15" s="30">
-        <v>3</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>5</v>
-      </c>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="4" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1190,10 +1213,10 @@
       <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="15.75">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1203,10 +1226,10 @@
       <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="15.75">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="6" t="s">
-        <v>15</v>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1216,10 +1239,10 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="7" t="s">
-        <v>16</v>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1229,10 +1252,10 @@
       <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="8" t="s">
-        <v>18</v>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1242,10 +1265,10 @@
       <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="8" t="s">
-        <v>19</v>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1255,10 +1278,10 @@
       <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="8" t="s">
-        <v>20</v>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1268,10 +1291,10 @@
       <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="7" t="s">
-        <v>21</v>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1281,23 +1304,35 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="8" t="s">
-        <v>23</v>
+      <c r="A24" s="27">
+        <v>3</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1307,10 +1342,10 @@
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="8" t="s">
-        <v>24</v>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1320,10 +1355,10 @@
       <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="9" t="s">
-        <v>25</v>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1333,14 +1368,10 @@
       <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="27">
-        <v>4</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>26</v>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1350,10 +1381,10 @@
       <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" ht="15.75">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="4" t="s">
-        <v>50</v>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1363,10 +1394,10 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="10" t="s">
-        <v>51</v>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1376,10 +1407,10 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" ht="15.75">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="11" t="s">
-        <v>52</v>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1389,10 +1420,10 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="11" t="s">
-        <v>53</v>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1402,10 +1433,10 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="12" t="s">
-        <v>27</v>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1415,10 +1446,10 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="10" t="s">
-        <v>28</v>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1428,10 +1459,10 @@
       <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="11" t="s">
-        <v>29</v>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1441,10 +1472,10 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="11" t="s">
-        <v>30</v>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1454,10 +1485,14 @@
       <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" ht="15.75">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="13" t="s">
-        <v>31</v>
+      <c r="A36" s="31">
+        <v>4</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1467,10 +1502,10 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="8" t="s">
-        <v>47</v>
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1480,10 +1515,10 @@
       <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="8" t="s">
-        <v>48</v>
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1493,10 +1528,10 @@
       <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="8" t="s">
-        <v>49</v>
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1506,10 +1541,10 @@
       <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="13" t="s">
-        <v>45</v>
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1519,10 +1554,10 @@
       <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="13" t="s">
-        <v>46</v>
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1532,14 +1567,10 @@
       <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="24">
-        <v>5</v>
-      </c>
-      <c r="B42" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>40</v>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1549,10 +1580,10 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="25"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="5" t="s">
-        <v>32</v>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1562,10 +1593,10 @@
       <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="25"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1575,10 +1606,10 @@
       <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="25"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="11" t="s">
-        <v>35</v>
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1588,10 +1619,10 @@
       <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="25"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="5" t="s">
-        <v>33</v>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1601,10 +1632,10 @@
       <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="25"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="11" t="s">
-        <v>34</v>
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1614,10 +1645,10 @@
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="25"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="11" t="s">
-        <v>35</v>
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1627,10 +1658,10 @@
       <c r="I48" s="15"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
-      <c r="A49" s="25"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="4" t="s">
-        <v>56</v>
+      <c r="A49" s="32"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1640,10 +1671,10 @@
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="25"/>
-      <c r="B50" s="30"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="13" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1653,10 +1684,14 @@
       <c r="I50" s="15"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
-      <c r="A51" s="25"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="11" t="s">
-        <v>17</v>
+      <c r="A51" s="28">
+        <v>5</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1666,10 +1701,10 @@
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
-      <c r="A52" s="25"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="11" t="s">
-        <v>38</v>
+      <c r="A52" s="29"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1679,10 +1714,10 @@
       <c r="I52" s="15"/>
     </row>
     <row r="53" spans="1:9" ht="15.75">
-      <c r="A53" s="25"/>
-      <c r="B53" s="30"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1692,10 +1727,10 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
-      <c r="A54" s="25"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="13" t="s">
-        <v>37</v>
+      <c r="A54" s="29"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1705,10 +1740,10 @@
       <c r="I54" s="15"/>
     </row>
     <row r="55" spans="1:9" ht="15.75">
-      <c r="A55" s="25"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="11" t="s">
-        <v>17</v>
+      <c r="A55" s="29"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1718,10 +1753,10 @@
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" ht="15.75">
-      <c r="A56" s="25"/>
-      <c r="B56" s="30"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1731,10 +1766,10 @@
       <c r="I56" s="15"/>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="25"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="13" t="s">
-        <v>54</v>
+      <c r="A57" s="29"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1744,10 +1779,10 @@
       <c r="I57" s="15"/>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="25"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="11" t="s">
-        <v>17</v>
+      <c r="A58" s="29"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1757,10 +1792,10 @@
       <c r="I58" s="15"/>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="26"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="11" t="s">
-        <v>38</v>
+      <c r="A59" s="29"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1770,14 +1805,10 @@
       <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="24">
-        <v>6</v>
-      </c>
-      <c r="B60" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>41</v>
+      <c r="A60" s="29"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1787,10 +1818,10 @@
       <c r="I60" s="15"/>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="25"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="13" t="s">
-        <v>42</v>
+      <c r="A61" s="29"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1800,10 +1831,10 @@
       <c r="I61" s="15"/>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="25"/>
-      <c r="B62" s="28"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="27"/>
       <c r="C62" s="11" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1813,10 +1844,10 @@
       <c r="I62" s="15"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="25"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="11" t="s">
-        <v>38</v>
+      <c r="A63" s="29"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1826,10 +1857,10 @@
       <c r="I63" s="15"/>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="25"/>
-      <c r="B64" s="28"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="27"/>
       <c r="C64" s="11" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -1839,10 +1870,10 @@
       <c r="I64" s="15"/>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="26"/>
-      <c r="B65" s="29"/>
-      <c r="C65" s="13" t="s">
-        <v>43</v>
+      <c r="A65" s="29"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -1851,132 +1882,131 @@
       <c r="H65" s="15"/>
       <c r="I65" s="15"/>
     </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="I66" s="3"/>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="I67" s="3"/>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:9" ht="60">
-      <c r="A69" s="21">
-        <v>1</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C69" s="4">
-        <v>1</v>
-      </c>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="I69" s="3"/>
-    </row>
-    <row r="70" spans="1:9" ht="30">
-      <c r="A70" s="23">
-        <v>2</v>
-      </c>
-      <c r="B70" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C70" s="23">
-        <v>2</v>
-      </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="1:9" ht="30">
-      <c r="A71" s="23">
-        <v>3</v>
-      </c>
-      <c r="B71" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="23">
-        <v>3</v>
-      </c>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:9" ht="30">
-      <c r="A72" s="23">
-        <v>4</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C72" s="23">
-        <v>4</v>
-      </c>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="1:9" ht="30">
-      <c r="A73" s="23">
-        <v>5</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C73" s="23">
-        <v>5</v>
-      </c>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="I73" s="3"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="I74" s="3"/>
+    <row r="66" spans="1:9" ht="15.75">
+      <c r="A66" s="29"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+    </row>
+    <row r="67" spans="1:9" ht="15.75">
+      <c r="A67" s="29"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" spans="1:9" ht="15.75">
+      <c r="A68" s="30"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" spans="1:9" ht="15.75">
+      <c r="A69" s="28">
+        <v>6</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" spans="1:9" ht="15.75">
+      <c r="A70" s="29"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" spans="1:9" ht="15.75">
+      <c r="A71" s="29"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75">
+      <c r="A72" s="29"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+    </row>
+    <row r="73" spans="1:9" ht="15.75">
+      <c r="A73" s="29"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+    </row>
+    <row r="74" spans="1:9" ht="15.75">
+      <c r="A74" s="30"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
     </row>
     <row r="75" spans="1:9">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="1"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -1984,6 +2014,11 @@
       <c r="I75" s="3"/>
     </row>
     <row r="76" spans="1:9">
+      <c r="A76" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="1"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -1991,106 +2026,223 @@
       <c r="I76" s="3"/>
     </row>
     <row r="77" spans="1:9">
+      <c r="A77" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="I77" s="3"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" ht="60">
+      <c r="A78" s="21">
+        <v>1</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1</v>
+      </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="I78" s="3"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" ht="30">
+      <c r="A79" s="23">
+        <v>2</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" s="23">
+        <v>2</v>
+      </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="I79" s="3"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" ht="30">
+      <c r="A80" s="23">
+        <v>3</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" s="23">
+        <v>3</v>
+      </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="I80" s="3"/>
     </row>
-    <row r="81" spans="4:9">
+    <row r="81" spans="1:9" ht="30">
+      <c r="A81" s="23">
+        <v>4</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" s="23">
+        <v>4</v>
+      </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="I81" s="3"/>
     </row>
-    <row r="82" spans="4:9">
+    <row r="82" spans="1:9" ht="30">
+      <c r="A82" s="23">
+        <v>5</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" s="23">
+        <v>5</v>
+      </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="I82" s="3"/>
     </row>
-    <row r="83" spans="4:9">
+    <row r="83" spans="1:9">
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="I83" s="3"/>
     </row>
-    <row r="84" spans="4:9">
+    <row r="84" spans="1:9">
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="I84" s="3"/>
     </row>
-    <row r="85" spans="4:9">
+    <row r="85" spans="1:9">
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="I85" s="3"/>
     </row>
-    <row r="86" spans="4:9">
+    <row r="86" spans="1:9">
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="I86" s="3"/>
     </row>
-    <row r="87" spans="4:9">
+    <row r="87" spans="1:9">
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="I87" s="3"/>
     </row>
-    <row r="88" spans="4:9">
+    <row r="88" spans="1:9">
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="I88" s="3"/>
     </row>
+    <row r="89" spans="1:9">
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="I89" s="3"/>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="I90" s="3"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="I91" s="3"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="I92" s="3"/>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="I93" s="3"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="I94" s="3"/>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="I95" s="3"/>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="I96" s="3"/>
+    </row>
+    <row r="97" spans="4:9">
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="I97" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="B51:B68"/>
+    <mergeCell ref="A51:A68"/>
+    <mergeCell ref="B36:B50"/>
+    <mergeCell ref="A36:A50"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A60:A65"/>
-    <mergeCell ref="B60:B65"/>
-    <mergeCell ref="B42:B59"/>
-    <mergeCell ref="A42:A59"/>
-    <mergeCell ref="B27:B41"/>
-    <mergeCell ref="A27:A41"/>
+    <mergeCell ref="B10:B23"/>
+    <mergeCell ref="B24:B35"/>
+    <mergeCell ref="A24:A35"/>
+    <mergeCell ref="A10:A23"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G86">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G95">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update tasksheet report 2
</commit_message>
<xml_diff>
--- a/Documents/C2B_TasksheetFinal.xlsx
+++ b/Documents/C2B_TasksheetFinal.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
   <si>
     <t>No.</t>
   </si>
@@ -611,12 +611,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,6 +624,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -940,7 +940,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -983,10 +983,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="26">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -1002,8 +1002,8 @@
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="4" t="s">
         <v>70</v>
       </c>
@@ -1017,8 +1017,8 @@
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="4" t="s">
         <v>71</v>
       </c>
@@ -1034,8 +1034,8 @@
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
@@ -1051,8 +1051,8 @@
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="4" t="s">
         <v>72</v>
       </c>
@@ -1072,8 +1072,8 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1093,8 +1093,8 @@
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="24" t="s">
         <v>73</v>
       </c>
@@ -1110,8 +1110,8 @@
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="25" t="s">
         <v>75</v>
       </c>
@@ -1131,172 +1131,222 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="27">
+      <c r="A10" s="32">
         <v>2</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="15.75">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="15.75">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="15.75">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15.75">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="15.75">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="15.75">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1304,8 +1354,8 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="4" t="s">
         <v>82</v>
       </c>
@@ -1325,10 +1375,10 @@
       <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="27">
+      <c r="A24" s="32">
         <v>3</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="32" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -1342,8 +1392,8 @@
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
@@ -1355,8 +1405,8 @@
       <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="6" t="s">
         <v>14</v>
       </c>
@@ -1368,8 +1418,8 @@
       <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="7" t="s">
         <v>15</v>
       </c>
@@ -1381,8 +1431,8 @@
       <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" ht="15.75">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="8" t="s">
         <v>17</v>
       </c>
@@ -1394,8 +1444,8 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="8" t="s">
         <v>18</v>
       </c>
@@ -1407,8 +1457,8 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" ht="15.75">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="8" t="s">
         <v>19</v>
       </c>
@@ -1420,8 +1470,8 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="7" t="s">
         <v>20</v>
       </c>
@@ -1433,8 +1483,8 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="8" t="s">
         <v>21</v>
       </c>
@@ -1446,8 +1496,8 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="8" t="s">
         <v>22</v>
       </c>
@@ -1459,8 +1509,8 @@
       <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="8" t="s">
         <v>23</v>
       </c>
@@ -1472,8 +1522,8 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="9" t="s">
         <v>24</v>
       </c>
@@ -1485,10 +1535,10 @@
       <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" ht="15.75">
-      <c r="A36" s="31">
+      <c r="A36" s="29">
         <v>4</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -1502,8 +1552,8 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
@@ -1515,8 +1565,8 @@
       <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="10" t="s">
         <v>50</v>
       </c>
@@ -1528,8 +1578,8 @@
       <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="32"/>
-      <c r="B39" s="32"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="11" t="s">
         <v>51</v>
       </c>
@@ -1541,8 +1591,8 @@
       <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="32"/>
-      <c r="B40" s="32"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="11" t="s">
         <v>52</v>
       </c>
@@ -1554,8 +1604,8 @@
       <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="32"/>
-      <c r="B41" s="32"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="12" t="s">
         <v>26</v>
       </c>
@@ -1567,8 +1617,8 @@
       <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="10" t="s">
         <v>27</v>
       </c>
@@ -1580,8 +1630,8 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="32"/>
-      <c r="B43" s="32"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="11" t="s">
         <v>28</v>
       </c>
@@ -1593,8 +1643,8 @@
       <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="32"/>
-      <c r="B44" s="32"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="11" t="s">
         <v>29</v>
       </c>
@@ -1606,8 +1656,8 @@
       <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="32"/>
-      <c r="B45" s="32"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="13" t="s">
         <v>30</v>
       </c>
@@ -1619,8 +1669,8 @@
       <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="8" t="s">
         <v>46</v>
       </c>
@@ -1632,8 +1682,8 @@
       <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="8" t="s">
         <v>47</v>
       </c>
@@ -1645,8 +1695,8 @@
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="8" t="s">
         <v>48</v>
       </c>
@@ -1658,8 +1708,8 @@
       <c r="I48" s="15"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="13" t="s">
         <v>44</v>
       </c>
@@ -1671,8 +1721,8 @@
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="13" t="s">
         <v>45</v>
       </c>
@@ -1684,10 +1734,10 @@
       <c r="I50" s="15"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
-      <c r="A51" s="28">
+      <c r="A51" s="26">
         <v>5</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="32" t="s">
         <v>54</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -1701,8 +1751,8 @@
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
-      <c r="A52" s="29"/>
-      <c r="B52" s="27"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="5" t="s">
         <v>31</v>
       </c>
@@ -1714,8 +1764,8 @@
       <c r="I52" s="15"/>
     </row>
     <row r="53" spans="1:9" ht="15.75">
-      <c r="A53" s="29"/>
-      <c r="B53" s="27"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="32"/>
       <c r="C53" s="11" t="s">
         <v>33</v>
       </c>
@@ -1727,8 +1777,8 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
-      <c r="A54" s="29"/>
-      <c r="B54" s="27"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="32"/>
       <c r="C54" s="11" t="s">
         <v>34</v>
       </c>
@@ -1740,8 +1790,8 @@
       <c r="I54" s="15"/>
     </row>
     <row r="55" spans="1:9" ht="15.75">
-      <c r="A55" s="29"/>
-      <c r="B55" s="27"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="32"/>
       <c r="C55" s="5" t="s">
         <v>32</v>
       </c>
@@ -1753,8 +1803,8 @@
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" ht="15.75">
-      <c r="A56" s="29"/>
-      <c r="B56" s="27"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="32"/>
       <c r="C56" s="11" t="s">
         <v>33</v>
       </c>
@@ -1766,8 +1816,8 @@
       <c r="I56" s="15"/>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="29"/>
-      <c r="B57" s="27"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="32"/>
       <c r="C57" s="11" t="s">
         <v>34</v>
       </c>
@@ -1779,8 +1829,8 @@
       <c r="I57" s="15"/>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="29"/>
-      <c r="B58" s="27"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="32"/>
       <c r="C58" s="4" t="s">
         <v>55</v>
       </c>
@@ -1792,8 +1842,8 @@
       <c r="I58" s="15"/>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="29"/>
-      <c r="B59" s="27"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="32"/>
       <c r="C59" s="13" t="s">
         <v>35</v>
       </c>
@@ -1805,8 +1855,8 @@
       <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="29"/>
-      <c r="B60" s="27"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="32"/>
       <c r="C60" s="11" t="s">
         <v>16</v>
       </c>
@@ -1818,8 +1868,8 @@
       <c r="I60" s="15"/>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="29"/>
-      <c r="B61" s="27"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="32"/>
       <c r="C61" s="11" t="s">
         <v>37</v>
       </c>
@@ -1831,8 +1881,8 @@
       <c r="I61" s="15"/>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="29"/>
-      <c r="B62" s="27"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="32"/>
       <c r="C62" s="11" t="s">
         <v>38</v>
       </c>
@@ -1844,8 +1894,8 @@
       <c r="I62" s="15"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="29"/>
-      <c r="B63" s="27"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="32"/>
       <c r="C63" s="13" t="s">
         <v>36</v>
       </c>
@@ -1857,8 +1907,8 @@
       <c r="I63" s="15"/>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="29"/>
-      <c r="B64" s="27"/>
+      <c r="A64" s="27"/>
+      <c r="B64" s="32"/>
       <c r="C64" s="11" t="s">
         <v>16</v>
       </c>
@@ -1870,8 +1920,8 @@
       <c r="I64" s="15"/>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="29"/>
-      <c r="B65" s="27"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="32"/>
       <c r="C65" s="11" t="s">
         <v>37</v>
       </c>
@@ -1883,8 +1933,8 @@
       <c r="I65" s="15"/>
     </row>
     <row r="66" spans="1:9" ht="15.75">
-      <c r="A66" s="29"/>
-      <c r="B66" s="27"/>
+      <c r="A66" s="27"/>
+      <c r="B66" s="32"/>
       <c r="C66" s="13" t="s">
         <v>53</v>
       </c>
@@ -1896,8 +1946,8 @@
       <c r="I66" s="15"/>
     </row>
     <row r="67" spans="1:9" ht="15.75">
-      <c r="A67" s="29"/>
-      <c r="B67" s="27"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="32"/>
       <c r="C67" s="11" t="s">
         <v>16</v>
       </c>
@@ -1909,8 +1959,8 @@
       <c r="I67" s="15"/>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="30"/>
-      <c r="B68" s="27"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="32"/>
       <c r="C68" s="11" t="s">
         <v>37</v>
       </c>
@@ -1922,10 +1972,10 @@
       <c r="I68" s="15"/>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="28">
+      <c r="A69" s="26">
         <v>6</v>
       </c>
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="13" t="s">
@@ -1939,8 +1989,8 @@
       <c r="I69" s="15"/>
     </row>
     <row r="70" spans="1:9" ht="15.75">
-      <c r="A70" s="29"/>
-      <c r="B70" s="32"/>
+      <c r="A70" s="27"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="13" t="s">
         <v>41</v>
       </c>
@@ -1952,8 +2002,8 @@
       <c r="I70" s="15"/>
     </row>
     <row r="71" spans="1:9" ht="15.75">
-      <c r="A71" s="29"/>
-      <c r="B71" s="32"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="30"/>
       <c r="C71" s="11" t="s">
         <v>16</v>
       </c>
@@ -1965,8 +2015,8 @@
       <c r="I71" s="15"/>
     </row>
     <row r="72" spans="1:9" ht="15.75">
-      <c r="A72" s="29"/>
-      <c r="B72" s="32"/>
+      <c r="A72" s="27"/>
+      <c r="B72" s="30"/>
       <c r="C72" s="11" t="s">
         <v>37</v>
       </c>
@@ -1978,8 +2028,8 @@
       <c r="I72" s="15"/>
     </row>
     <row r="73" spans="1:9" ht="15.75">
-      <c r="A73" s="29"/>
-      <c r="B73" s="32"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="30"/>
       <c r="C73" s="11" t="s">
         <v>38</v>
       </c>
@@ -1991,8 +2041,8 @@
       <c r="I73" s="15"/>
     </row>
     <row r="74" spans="1:9" ht="15.75">
-      <c r="A74" s="30"/>
-      <c r="B74" s="26"/>
+      <c r="A74" s="28"/>
+      <c r="B74" s="31"/>
       <c r="C74" s="13" t="s">
         <v>42</v>
       </c>
@@ -2228,18 +2278,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B10:B23"/>
+    <mergeCell ref="B24:B35"/>
+    <mergeCell ref="A24:A35"/>
+    <mergeCell ref="A10:A23"/>
     <mergeCell ref="A69:A74"/>
     <mergeCell ref="B69:B74"/>
     <mergeCell ref="B51:B68"/>
     <mergeCell ref="A51:A68"/>
     <mergeCell ref="B36:B50"/>
     <mergeCell ref="A36:A50"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B10:B23"/>
-    <mergeCell ref="B24:B35"/>
-    <mergeCell ref="A24:A35"/>
-    <mergeCell ref="A10:A23"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G95">

</xml_diff>

<commit_message>
Update task sheet + Report 3 template
</commit_message>
<xml_diff>
--- a/Documents/C2B_TasksheetFinal.xlsx
+++ b/Documents/C2B_TasksheetFinal.xlsx
@@ -74,60 +74,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C25" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Use bold format for tasks which have sub-tasks</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C26" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Use Indent for sub-tasks</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="126">
   <si>
     <t>No.</t>
   </si>
@@ -180,15 +132,6 @@
     <t>Function 1</t>
   </si>
   <si>
-    <t>Function 1 (Usecase &amp; Usecase Specification)</t>
-  </si>
-  <si>
-    <t>Function 2 (Usecase &amp; Usecase Specification)</t>
-  </si>
-  <si>
-    <t>Function n (Usecase &amp; Usecase Specification)</t>
-  </si>
-  <si>
     <t>Non-functional Requirement</t>
   </si>
   <si>
@@ -198,9 +141,6 @@
     <t>Availability</t>
   </si>
   <si>
-    <t>…….</t>
-  </si>
-  <si>
     <t>Entity Relationship Diagram</t>
   </si>
   <si>
@@ -357,41 +297,173 @@
     <t>Review Report 1</t>
   </si>
   <si>
-    <t>_Name of this Capstone Project</t>
-  </si>
-  <si>
-    <t>_Problem Abstract</t>
-  </si>
-  <si>
-    <t>_Project Overview</t>
-  </si>
-  <si>
-    <t>_Software Process Model</t>
-  </si>
-  <si>
-    <t>_Roles and responsibilities</t>
-  </si>
-  <si>
-    <t>_Tools and Techniques</t>
-  </si>
-  <si>
     <t>Review Report 2</t>
   </si>
   <si>
-    <t>_Software development life cycle</t>
-  </si>
-  <si>
-    <t>_Phase Detail</t>
-  </si>
-  <si>
-    <t>_All Meeting Minutes</t>
+    <t>Name of this Capstone Project</t>
+  </si>
+  <si>
+    <t>Problem Abstract</t>
+  </si>
+  <si>
+    <t>Project Overview</t>
+  </si>
+  <si>
+    <t>Software Process Model</t>
+  </si>
+  <si>
+    <t>Roles and responsibilities</t>
+  </si>
+  <si>
+    <t>Tools and Techniques</t>
+  </si>
+  <si>
+    <t>Software development life cycle</t>
+  </si>
+  <si>
+    <t>Phase Detail</t>
+  </si>
+  <si>
+    <t>All Meeting Minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Requirement </t>
+  </si>
+  <si>
+    <t>Customer Requirement</t>
+  </si>
+  <si>
+    <t>Supplier Requirement</t>
+  </si>
+  <si>
+    <t>Admin Requirement</t>
+  </si>
+  <si>
+    <t>Guest Requirement</t>
+  </si>
+  <si>
+    <t>System Overview Use Case</t>
+  </si>
+  <si>
+    <t>List of Use Case</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Maintainability</t>
+  </si>
+  <si>
+    <t>Portability</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Review Report 3</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>View Shop</t>
+  </si>
+  <si>
+    <t>Search Shop</t>
+  </si>
+  <si>
+    <t>View Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat </t>
+  </si>
+  <si>
+    <t>Manage Request</t>
+  </si>
+  <si>
+    <t>Create Request</t>
+  </si>
+  <si>
+    <t>Cancel Request</t>
+  </si>
+  <si>
+    <t>Select Supplier</t>
+  </si>
+  <si>
+    <t>Send Feedback</t>
+  </si>
+  <si>
+    <t>Edit Profile</t>
+  </si>
+  <si>
+    <t>Post Bid</t>
+  </si>
+  <si>
+    <t>View Bid</t>
+  </si>
+  <si>
+    <t>Search Bid</t>
+  </si>
+  <si>
+    <t>Confirm Order</t>
+  </si>
+  <si>
+    <t>Choose Payment</t>
+  </si>
+  <si>
+    <t>View Order</t>
+  </si>
+  <si>
+    <t>Search Order</t>
+  </si>
+  <si>
+    <t>Review Shop</t>
+  </si>
+  <si>
+    <t>Manage Shop</t>
+  </si>
+  <si>
+    <t>Create Shop</t>
+  </si>
+  <si>
+    <t>Edit Shop</t>
+  </si>
+  <si>
+    <t>View Shop's Product</t>
+  </si>
+  <si>
+    <t>Search Shop's Product</t>
+  </si>
+  <si>
+    <t>Edit Shop's Product</t>
+  </si>
+  <si>
+    <t>Add Shop's Product</t>
+  </si>
+  <si>
+    <t>Delete Shop's Product</t>
+  </si>
+  <si>
+    <t>Reply Request</t>
+  </si>
+  <si>
+    <t>View Bid's History</t>
+  </si>
+  <si>
+    <t>Retract</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +535,21 @@
       <color indexed="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="5">
@@ -556,7 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -611,6 +698,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -626,11 +719,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -937,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -964,36 +1058,36 @@
         <v>2</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="31">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1002,13 +1096,13 @@
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1017,16 +1111,16 @@
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1034,117 +1128,117 @@
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="32">
+      <c r="A10" s="27">
         <v>2</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1152,50 +1246,50 @@
       <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="4" t="s">
-        <v>76</v>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="35" t="s">
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="15.75">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="4" t="s">
-        <v>77</v>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="15.75">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="4" t="s">
-        <v>78</v>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1203,84 +1297,84 @@
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="15.75">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15.75">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="4" t="s">
-        <v>79</v>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" ht="15.75">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="4" t="s">
-        <v>80</v>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="35" t="s">
+        <v>77</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="15.75">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="4" t="s">
-        <v>81</v>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="35" t="s">
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1288,16 +1382,16 @@
       <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="4" t="s">
-        <v>83</v>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="35" t="s">
+        <v>79</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1305,47 +1399,47 @@
       <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="4" t="s">
-        <v>84</v>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="35" t="s">
+        <v>80</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="4" t="s">
-        <v>85</v>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="35" t="s">
+        <v>81</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1354,34 +1448,34 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="32">
+      <c r="A24" s="27">
         <v>3</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="33" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="2"/>
@@ -1392,10 +1486,10 @@
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="5" t="s">
-        <v>13</v>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="34" t="s">
+        <v>86</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1405,10 +1499,10 @@
       <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="6" t="s">
-        <v>14</v>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="34" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1418,10 +1512,10 @@
       <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="7" t="s">
-        <v>15</v>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="34" t="s">
+        <v>83</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1431,10 +1525,10 @@
       <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" ht="15.75">
-      <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="8" t="s">
-        <v>17</v>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="34" t="s">
+        <v>84</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1444,10 +1538,10 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="8" t="s">
-        <v>18</v>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="34" t="s">
+        <v>85</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1457,10 +1551,10 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" ht="15.75">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="8" t="s">
-        <v>19</v>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1470,10 +1564,10 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="7" t="s">
-        <v>20</v>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1483,10 +1577,10 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="8" t="s">
-        <v>21</v>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1496,10 +1590,10 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="8" t="s">
-        <v>22</v>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1509,10 +1603,10 @@
       <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="8" t="s">
-        <v>23</v>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1522,10 +1616,10 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="9" t="s">
-        <v>24</v>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1535,14 +1629,10 @@
       <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" ht="15.75">
-      <c r="A36" s="29">
-        <v>4</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>25</v>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1552,10 +1642,10 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="4" t="s">
-        <v>49</v>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1565,10 +1655,10 @@
       <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="10" t="s">
-        <v>50</v>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1578,10 +1668,10 @@
       <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="11" t="s">
-        <v>51</v>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1591,10 +1681,10 @@
       <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="11" t="s">
-        <v>52</v>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1604,10 +1694,10 @@
       <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="12" t="s">
-        <v>26</v>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1617,10 +1707,10 @@
       <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="10" t="s">
-        <v>27</v>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1630,10 +1720,10 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="11" t="s">
-        <v>28</v>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1643,10 +1733,10 @@
       <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="11" t="s">
-        <v>29</v>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1656,10 +1746,10 @@
       <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="13" t="s">
-        <v>30</v>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1669,10 +1759,10 @@
       <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="8" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1682,10 +1772,10 @@
       <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1695,10 +1785,10 @@
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="8" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1708,10 +1798,10 @@
       <c r="I48" s="15"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="13" t="s">
-        <v>44</v>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1721,10 +1811,10 @@
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="13" t="s">
-        <v>45</v>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1734,14 +1824,10 @@
       <c r="I50" s="15"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
-      <c r="A51" s="26">
-        <v>5</v>
-      </c>
-      <c r="B51" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>39</v>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1752,9 +1838,9 @@
     </row>
     <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="27"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="5" t="s">
-        <v>31</v>
+      <c r="B52" s="27"/>
+      <c r="C52" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1765,9 +1851,9 @@
     </row>
     <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="27"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="11" t="s">
-        <v>33</v>
+      <c r="B53" s="27"/>
+      <c r="C53" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1778,9 +1864,9 @@
     </row>
     <row r="54" spans="1:9" ht="15.75">
       <c r="A54" s="27"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="11" t="s">
-        <v>34</v>
+      <c r="B54" s="27"/>
+      <c r="C54" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1791,9 +1877,9 @@
     </row>
     <row r="55" spans="1:9" ht="15.75">
       <c r="A55" s="27"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="5" t="s">
-        <v>32</v>
+      <c r="B55" s="27"/>
+      <c r="C55" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1804,9 +1890,9 @@
     </row>
     <row r="56" spans="1:9" ht="15.75">
       <c r="A56" s="27"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="11" t="s">
-        <v>33</v>
+      <c r="B56" s="27"/>
+      <c r="C56" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1817,9 +1903,9 @@
     </row>
     <row r="57" spans="1:9" ht="15.75">
       <c r="A57" s="27"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="11" t="s">
-        <v>34</v>
+      <c r="B57" s="27"/>
+      <c r="C57" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1830,9 +1916,9 @@
     </row>
     <row r="58" spans="1:9" ht="15.75">
       <c r="A58" s="27"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="4" t="s">
-        <v>55</v>
+      <c r="B58" s="27"/>
+      <c r="C58" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1843,9 +1929,9 @@
     </row>
     <row r="59" spans="1:9" ht="15.75">
       <c r="A59" s="27"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="13" t="s">
-        <v>35</v>
+      <c r="B59" s="27"/>
+      <c r="C59" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1856,9 +1942,9 @@
     </row>
     <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="27"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="11" t="s">
-        <v>16</v>
+      <c r="B60" s="27"/>
+      <c r="C60" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1869,9 +1955,9 @@
     </row>
     <row r="61" spans="1:9" ht="15.75">
       <c r="A61" s="27"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="11" t="s">
-        <v>37</v>
+      <c r="B61" s="27"/>
+      <c r="C61" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1882,9 +1968,9 @@
     </row>
     <row r="62" spans="1:9" ht="15.75">
       <c r="A62" s="27"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="11" t="s">
-        <v>38</v>
+      <c r="B62" s="27"/>
+      <c r="C62" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1895,9 +1981,9 @@
     </row>
     <row r="63" spans="1:9" ht="15.75">
       <c r="A63" s="27"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="13" t="s">
-        <v>36</v>
+      <c r="B63" s="27"/>
+      <c r="C63" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1908,9 +1994,9 @@
     </row>
     <row r="64" spans="1:9" ht="15.75">
       <c r="A64" s="27"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="11" t="s">
-        <v>16</v>
+      <c r="B64" s="27"/>
+      <c r="C64" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -1921,9 +2007,9 @@
     </row>
     <row r="65" spans="1:9" ht="15.75">
       <c r="A65" s="27"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="11" t="s">
-        <v>37</v>
+      <c r="B65" s="27"/>
+      <c r="C65" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -1934,10 +2020,8 @@
     </row>
     <row r="66" spans="1:9" ht="15.75">
       <c r="A66" s="27"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="13" t="s">
-        <v>53</v>
-      </c>
+      <c r="B66" s="27"/>
+      <c r="C66" s="8"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -1947,10 +2031,8 @@
     </row>
     <row r="67" spans="1:9" ht="15.75">
       <c r="A67" s="27"/>
-      <c r="B67" s="32"/>
-      <c r="C67" s="11" t="s">
-        <v>16</v>
-      </c>
+      <c r="B67" s="27"/>
+      <c r="C67" s="8"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -1959,11 +2041,9 @@
       <c r="I67" s="15"/>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="28"/>
-      <c r="B68" s="32"/>
-      <c r="C68" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="8"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -1972,15 +2052,9 @@
       <c r="I68" s="15"/>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="26">
-        <v>6</v>
-      </c>
-      <c r="B69" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="8"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -1990,10 +2064,8 @@
     </row>
     <row r="70" spans="1:9" ht="15.75">
       <c r="A70" s="27"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="B70" s="27"/>
+      <c r="C70" s="8"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -2003,10 +2075,8 @@
     </row>
     <row r="71" spans="1:9" ht="15.75">
       <c r="A71" s="27"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="11" t="s">
-        <v>16</v>
-      </c>
+      <c r="B71" s="27"/>
+      <c r="C71" s="8"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2016,10 +2086,8 @@
     </row>
     <row r="72" spans="1:9" ht="15.75">
       <c r="A72" s="27"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="B72" s="27"/>
+      <c r="C72" s="8"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -2029,10 +2097,8 @@
     </row>
     <row r="73" spans="1:9" ht="15.75">
       <c r="A73" s="27"/>
-      <c r="B73" s="30"/>
-      <c r="C73" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="B73" s="27"/>
+      <c r="C73" s="8"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2041,11 +2107,9 @@
       <c r="I73" s="15"/>
     </row>
     <row r="74" spans="1:9" ht="15.75">
-      <c r="A74" s="28"/>
-      <c r="B74" s="31"/>
-      <c r="C74" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="8"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2053,246 +2117,1178 @@
       <c r="H74" s="15"/>
       <c r="I74" s="15"/>
     </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="20" t="s">
+    <row r="75" spans="1:9" ht="15.75">
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+    </row>
+    <row r="76" spans="1:9" ht="15.75">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+    </row>
+    <row r="77" spans="1:9" ht="15.75">
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+    </row>
+    <row r="78" spans="1:9" ht="15.75">
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+    </row>
+    <row r="79" spans="1:9" ht="15.75">
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+    </row>
+    <row r="80" spans="1:9" ht="15.75">
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+    </row>
+    <row r="81" spans="1:9" ht="15.75">
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+    </row>
+    <row r="82" spans="1:9" ht="15.75">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+    </row>
+    <row r="83" spans="1:9" ht="15.75">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+    </row>
+    <row r="84" spans="1:9" ht="15.75">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+    </row>
+    <row r="85" spans="1:9" ht="15.75">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+    </row>
+    <row r="86" spans="1:9" ht="15.75">
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+    </row>
+    <row r="87" spans="1:9" ht="15.75">
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+    </row>
+    <row r="88" spans="1:9" ht="15.75">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+    </row>
+    <row r="89" spans="1:9" ht="15.75">
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+    </row>
+    <row r="90" spans="1:9" ht="15.75">
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
+    </row>
+    <row r="91" spans="1:9" ht="15.75">
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+    </row>
+    <row r="92" spans="1:9" ht="15.75">
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+    </row>
+    <row r="93" spans="1:9" ht="15.75">
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+    </row>
+    <row r="94" spans="1:9" ht="15.75">
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
+    </row>
+    <row r="95" spans="1:9" ht="15.75">
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+    </row>
+    <row r="96" spans="1:9" ht="15.75">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+    </row>
+    <row r="97" spans="1:9" ht="15.75">
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+    </row>
+    <row r="98" spans="1:9" ht="15.75">
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+    </row>
+    <row r="99" spans="1:9" ht="15.75">
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+    </row>
+    <row r="100" spans="1:9" ht="15.75">
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15"/>
+    </row>
+    <row r="101" spans="1:9" ht="15.75">
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15"/>
+    </row>
+    <row r="102" spans="1:9" ht="15.75">
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="15"/>
+      <c r="I102" s="15"/>
+    </row>
+    <row r="103" spans="1:9" ht="15.75">
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="15"/>
+      <c r="I103" s="15"/>
+    </row>
+    <row r="104" spans="1:9" ht="15.75">
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
+      <c r="C104" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="15"/>
+      <c r="I104" s="15"/>
+    </row>
+    <row r="105" spans="1:9" ht="15.75">
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="15"/>
+      <c r="I105" s="15"/>
+    </row>
+    <row r="106" spans="1:9" ht="15.75">
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="15"/>
+      <c r="I106" s="15"/>
+    </row>
+    <row r="107" spans="1:9" ht="15.75">
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="15"/>
+      <c r="I107" s="15"/>
+    </row>
+    <row r="108" spans="1:9" ht="15.75">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="15"/>
+      <c r="I108" s="15"/>
+    </row>
+    <row r="109" spans="1:9" ht="15.75">
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H109" s="15"/>
+      <c r="I109" s="15"/>
+    </row>
+    <row r="110" spans="1:9" ht="15.75">
+      <c r="A110" s="31">
+        <v>4</v>
+      </c>
+      <c r="B110" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="15"/>
+      <c r="I110" s="15"/>
+    </row>
+    <row r="111" spans="1:9" ht="15.75">
+      <c r="A111" s="32"/>
+      <c r="B111" s="32"/>
+      <c r="C111" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="15"/>
+      <c r="I111" s="15"/>
+    </row>
+    <row r="112" spans="1:9" ht="15.75">
+      <c r="A112" s="32"/>
+      <c r="B112" s="32"/>
+      <c r="C112" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="15"/>
+      <c r="I112" s="15"/>
+    </row>
+    <row r="113" spans="1:9" ht="15.75">
+      <c r="A113" s="32"/>
+      <c r="B113" s="32"/>
+      <c r="C113" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="15"/>
+      <c r="I113" s="15"/>
+    </row>
+    <row r="114" spans="1:9" ht="15.75">
+      <c r="A114" s="32"/>
+      <c r="B114" s="32"/>
+      <c r="C114" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="15"/>
+      <c r="I114" s="15"/>
+    </row>
+    <row r="115" spans="1:9" ht="15.75">
+      <c r="A115" s="32"/>
+      <c r="B115" s="32"/>
+      <c r="C115" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="15"/>
+      <c r="I115" s="15"/>
+    </row>
+    <row r="116" spans="1:9" ht="15.75">
+      <c r="A116" s="32"/>
+      <c r="B116" s="32"/>
+      <c r="C116" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="15"/>
+      <c r="I116" s="15"/>
+    </row>
+    <row r="117" spans="1:9" ht="15.75">
+      <c r="A117" s="32"/>
+      <c r="B117" s="32"/>
+      <c r="C117" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="15"/>
+      <c r="I117" s="15"/>
+    </row>
+    <row r="118" spans="1:9" ht="15.75">
+      <c r="A118" s="32"/>
+      <c r="B118" s="32"/>
+      <c r="C118" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="15"/>
+      <c r="I118" s="15"/>
+    </row>
+    <row r="119" spans="1:9" ht="15.75">
+      <c r="A119" s="32"/>
+      <c r="B119" s="32"/>
+      <c r="C119" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="15"/>
+      <c r="I119" s="15"/>
+    </row>
+    <row r="120" spans="1:9" ht="15.75">
+      <c r="A120" s="32"/>
+      <c r="B120" s="32"/>
+      <c r="C120" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="15"/>
+      <c r="I120" s="15"/>
+    </row>
+    <row r="121" spans="1:9" ht="15.75">
+      <c r="A121" s="32"/>
+      <c r="B121" s="32"/>
+      <c r="C121" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="15"/>
+      <c r="I121" s="15"/>
+    </row>
+    <row r="122" spans="1:9" ht="15.75">
+      <c r="A122" s="32"/>
+      <c r="B122" s="32"/>
+      <c r="C122" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="15"/>
+      <c r="I122" s="15"/>
+    </row>
+    <row r="123" spans="1:9" ht="15.75">
+      <c r="A123" s="32"/>
+      <c r="B123" s="32"/>
+      <c r="C123" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="15"/>
+      <c r="I123" s="15"/>
+    </row>
+    <row r="124" spans="1:9" ht="15.75">
+      <c r="A124" s="26"/>
+      <c r="B124" s="26"/>
+      <c r="C124" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="15"/>
+      <c r="I124" s="15"/>
+    </row>
+    <row r="125" spans="1:9" ht="15.75">
+      <c r="A125" s="28">
+        <v>5</v>
+      </c>
+      <c r="B125" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="15"/>
+      <c r="I125" s="15"/>
+    </row>
+    <row r="126" spans="1:9" ht="15.75">
+      <c r="A126" s="29"/>
+      <c r="B126" s="27"/>
+      <c r="C126" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="15"/>
+      <c r="I126" s="15"/>
+    </row>
+    <row r="127" spans="1:9" ht="15.75">
+      <c r="A127" s="29"/>
+      <c r="B127" s="27"/>
+      <c r="C127" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="15"/>
+      <c r="I127" s="15"/>
+    </row>
+    <row r="128" spans="1:9" ht="15.75">
+      <c r="A128" s="29"/>
+      <c r="B128" s="27"/>
+      <c r="C128" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="15"/>
+      <c r="I128" s="15"/>
+    </row>
+    <row r="129" spans="1:9" ht="15.75">
+      <c r="A129" s="29"/>
+      <c r="B129" s="27"/>
+      <c r="C129" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="15"/>
+      <c r="I129" s="15"/>
+    </row>
+    <row r="130" spans="1:9" ht="15.75">
+      <c r="A130" s="29"/>
+      <c r="B130" s="27"/>
+      <c r="C130" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="15"/>
+      <c r="I130" s="15"/>
+    </row>
+    <row r="131" spans="1:9" ht="15.75">
+      <c r="A131" s="29"/>
+      <c r="B131" s="27"/>
+      <c r="C131" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="15"/>
+      <c r="I131" s="15"/>
+    </row>
+    <row r="132" spans="1:9" ht="15.75">
+      <c r="A132" s="29"/>
+      <c r="B132" s="27"/>
+      <c r="C132" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="15"/>
+      <c r="I132" s="15"/>
+    </row>
+    <row r="133" spans="1:9" ht="15.75">
+      <c r="A133" s="29"/>
+      <c r="B133" s="27"/>
+      <c r="C133" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+      <c r="H133" s="15"/>
+      <c r="I133" s="15"/>
+    </row>
+    <row r="134" spans="1:9" ht="15.75">
+      <c r="A134" s="29"/>
+      <c r="B134" s="27"/>
+      <c r="C134" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="15"/>
+      <c r="I134" s="15"/>
+    </row>
+    <row r="135" spans="1:9" ht="15.75">
+      <c r="A135" s="29"/>
+      <c r="B135" s="27"/>
+      <c r="C135" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="15"/>
+      <c r="I135" s="15"/>
+    </row>
+    <row r="136" spans="1:9" ht="15.75">
+      <c r="A136" s="29"/>
+      <c r="B136" s="27"/>
+      <c r="C136" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="15"/>
+      <c r="I136" s="15"/>
+    </row>
+    <row r="137" spans="1:9" ht="15.75">
+      <c r="A137" s="29"/>
+      <c r="B137" s="27"/>
+      <c r="C137" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="15"/>
+      <c r="I137" s="15"/>
+    </row>
+    <row r="138" spans="1:9" ht="15.75">
+      <c r="A138" s="29"/>
+      <c r="B138" s="27"/>
+      <c r="C138" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="15"/>
+      <c r="I138" s="15"/>
+    </row>
+    <row r="139" spans="1:9" ht="15.75">
+      <c r="A139" s="29"/>
+      <c r="B139" s="27"/>
+      <c r="C139" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="15"/>
+      <c r="I139" s="15"/>
+    </row>
+    <row r="140" spans="1:9" ht="15.75">
+      <c r="A140" s="29"/>
+      <c r="B140" s="27"/>
+      <c r="C140" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="15"/>
+      <c r="I140" s="15"/>
+    </row>
+    <row r="141" spans="1:9" ht="15.75">
+      <c r="A141" s="29"/>
+      <c r="B141" s="27"/>
+      <c r="C141" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+      <c r="H141" s="15"/>
+      <c r="I141" s="15"/>
+    </row>
+    <row r="142" spans="1:9" ht="15.75">
+      <c r="A142" s="30"/>
+      <c r="B142" s="27"/>
+      <c r="C142" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="15"/>
+      <c r="I142" s="15"/>
+    </row>
+    <row r="143" spans="1:9" ht="15.75">
+      <c r="A143" s="28">
+        <v>6</v>
+      </c>
+      <c r="B143" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+      <c r="H143" s="15"/>
+      <c r="I143" s="15"/>
+    </row>
+    <row r="144" spans="1:9" ht="15.75">
+      <c r="A144" s="29"/>
+      <c r="B144" s="32"/>
+      <c r="C144" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="15"/>
+      <c r="I144" s="15"/>
+    </row>
+    <row r="145" spans="1:9" ht="15.75">
+      <c r="A145" s="29"/>
+      <c r="B145" s="32"/>
+      <c r="C145" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="15"/>
+      <c r="I145" s="15"/>
+    </row>
+    <row r="146" spans="1:9" ht="15.75">
+      <c r="A146" s="29"/>
+      <c r="B146" s="32"/>
+      <c r="C146" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="15"/>
+      <c r="I146" s="15"/>
+    </row>
+    <row r="147" spans="1:9" ht="15.75">
+      <c r="A147" s="29"/>
+      <c r="B147" s="32"/>
+      <c r="C147" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+      <c r="H147" s="15"/>
+      <c r="I147" s="15"/>
+    </row>
+    <row r="148" spans="1:9" ht="15.75">
+      <c r="A148" s="30"/>
+      <c r="B148" s="26"/>
+      <c r="C148" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+      <c r="H148" s="15"/>
+      <c r="I148" s="15"/>
+    </row>
+    <row r="149" spans="1:9">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
+      <c r="I149" s="3"/>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="A150" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B150" s="3"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
+      <c r="I150" s="3"/>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="A151" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B151" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D151" s="3"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="3"/>
+      <c r="G151" s="3"/>
+      <c r="I151" s="3"/>
+    </row>
+    <row r="152" spans="1:9" ht="60">
+      <c r="A152" s="21">
+        <v>1</v>
+      </c>
+      <c r="B152" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C152" s="4">
+        <v>1</v>
+      </c>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
+      <c r="I152" s="3"/>
+    </row>
+    <row r="153" spans="1:9" ht="30">
+      <c r="A153" s="23">
+        <v>2</v>
+      </c>
+      <c r="B153" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C153" s="23">
+        <v>2</v>
+      </c>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="3"/>
+      <c r="G153" s="3"/>
+      <c r="I153" s="3"/>
+    </row>
+    <row r="154" spans="1:9" ht="30">
+      <c r="A154" s="23">
+        <v>3</v>
+      </c>
+      <c r="B154" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="I76" s="3"/>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B77" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C77" s="4" t="s">
+      <c r="C154" s="23">
+        <v>3</v>
+      </c>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
+      <c r="I154" s="3"/>
+    </row>
+    <row r="155" spans="1:9" ht="30">
+      <c r="A155" s="23">
+        <v>4</v>
+      </c>
+      <c r="B155" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C155" s="23">
+        <v>4</v>
+      </c>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
+      <c r="I155" s="3"/>
+    </row>
+    <row r="156" spans="1:9" ht="30">
+      <c r="A156" s="23">
+        <v>5</v>
+      </c>
+      <c r="B156" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="I77" s="3"/>
-    </row>
-    <row r="78" spans="1:9" ht="60">
-      <c r="A78" s="21">
-        <v>1</v>
-      </c>
-      <c r="B78" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C78" s="4">
-        <v>1</v>
-      </c>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="I78" s="3"/>
-    </row>
-    <row r="79" spans="1:9" ht="30">
-      <c r="A79" s="23">
-        <v>2</v>
-      </c>
-      <c r="B79" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" s="23">
-        <v>2</v>
-      </c>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="I79" s="3"/>
-    </row>
-    <row r="80" spans="1:9" ht="30">
-      <c r="A80" s="23">
-        <v>3</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C80" s="23">
-        <v>3</v>
-      </c>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="I80" s="3"/>
-    </row>
-    <row r="81" spans="1:9" ht="30">
-      <c r="A81" s="23">
-        <v>4</v>
-      </c>
-      <c r="B81" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C81" s="23">
-        <v>4</v>
-      </c>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="I81" s="3"/>
-    </row>
-    <row r="82" spans="1:9" ht="30">
-      <c r="A82" s="23">
+      <c r="C156" s="23">
         <v>5</v>
       </c>
-      <c r="B82" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C82" s="23">
-        <v>5</v>
-      </c>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="I83" s="3"/>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="I85" s="3"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="I87" s="3"/>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="I89" s="3"/>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-      <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="I92" s="3"/>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-      <c r="I93" s="3"/>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="I94" s="3"/>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="I95" s="3"/>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="I96" s="3"/>
-    </row>
-    <row r="97" spans="4:9">
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
-      <c r="I97" s="3"/>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="3"/>
+      <c r="G156" s="3"/>
+      <c r="I156" s="3"/>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
+      <c r="I157" s="3"/>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
+      <c r="I158" s="3"/>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="D159" s="3"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3"/>
+      <c r="I159" s="3"/>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
+      <c r="I160" s="3"/>
+    </row>
+    <row r="161" spans="4:9">
+      <c r="D161" s="3"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3"/>
+      <c r="I161" s="3"/>
+    </row>
+    <row r="162" spans="4:9">
+      <c r="D162" s="3"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3"/>
+      <c r="I162" s="3"/>
+    </row>
+    <row r="163" spans="4:9">
+      <c r="D163" s="3"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+      <c r="I163" s="3"/>
+    </row>
+    <row r="164" spans="4:9">
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="3"/>
+      <c r="G164" s="3"/>
+      <c r="I164" s="3"/>
+    </row>
+    <row r="165" spans="4:9">
+      <c r="D165" s="3"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="3"/>
+      <c r="G165" s="3"/>
+      <c r="I165" s="3"/>
+    </row>
+    <row r="166" spans="4:9">
+      <c r="D166" s="3"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="3"/>
+      <c r="G166" s="3"/>
+      <c r="I166" s="3"/>
+    </row>
+    <row r="167" spans="4:9">
+      <c r="D167" s="3"/>
+      <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
+      <c r="I167" s="3"/>
+    </row>
+    <row r="168" spans="4:9">
+      <c r="D168" s="3"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="3"/>
+      <c r="G168" s="3"/>
+      <c r="I168" s="3"/>
+    </row>
+    <row r="169" spans="4:9">
+      <c r="D169" s="3"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+      <c r="G169" s="3"/>
+      <c r="I169" s="3"/>
+    </row>
+    <row r="170" spans="4:9">
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
+      <c r="I170" s="3"/>
+    </row>
+    <row r="171" spans="4:9">
+      <c r="D171" s="3"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
+      <c r="I171" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A143:A148"/>
+    <mergeCell ref="B143:B148"/>
+    <mergeCell ref="B125:B142"/>
+    <mergeCell ref="A125:A142"/>
+    <mergeCell ref="B110:B124"/>
+    <mergeCell ref="A110:A124"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B10:B23"/>
-    <mergeCell ref="B24:B35"/>
-    <mergeCell ref="A24:A35"/>
+    <mergeCell ref="B24:B109"/>
+    <mergeCell ref="A24:A109"/>
     <mergeCell ref="A10:A23"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="B69:B74"/>
-    <mergeCell ref="B51:B68"/>
-    <mergeCell ref="A51:A68"/>
-    <mergeCell ref="B36:B50"/>
-    <mergeCell ref="A36:A50"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G95">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G169">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>